<commit_message>
Data for Terr Herb Mammals
</commit_message>
<xml_diff>
--- a/data_impute_project/error_metrics/terrestrial_herbivorous_mammals/min_mae_mape_all_features_combined_terrestrial_herbivorous_mammals.xlsx
+++ b/data_impute_project/error_metrics/terrestrial_herbivorous_mammals/min_mae_mape_all_features_combined_terrestrial_herbivorous_mammals.xlsx
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_1_ABCD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -491,24 +491,20 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0.2985953968253966</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1.332453872828025</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_1_ABCD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -522,28 +518,24 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>ABCD</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.3007955555555555</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.350484907338554</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_1_ABCD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -557,28 +549,24 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="F4" t="n">
+        <v>0.373043180349063</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.672091178108411</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_3_ABCDF</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -596,24 +584,20 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_3_ABCDF</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -623,32 +607,28 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>RandomForest</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.008929999999998601</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1541971880261283</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_3_ABCDF</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -658,32 +638,28 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>RandomForest_MICE</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.1516413333333328</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.454008133207574</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_3_ABCDF</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -701,24 +677,20 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_3_ABCDF</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -728,32 +700,28 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>RandomForest_MICE</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>ABCD</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0394049999999994</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.369999999999995</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_3_ABCDF</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -763,32 +731,28 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>RandomForest_MICE</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>ABCD</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0111479999999996</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1046760563380243</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_3_ABCDF</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -806,18 +770,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -833,32 +793,28 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>RandomForest</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>BCDE</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0431080714285713</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.5039291049652861</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>combination_2_ABCDE</t>
+          <t>combination_3_ABCDF</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -868,26 +824,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>RandomForest_MICE</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>BCDF</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.094764</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.843657587548639</v>
       </c>
     </row>
     <row r="14">
@@ -911,18 +863,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>ACDE</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.00024</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0014388489208633</v>
       </c>
     </row>
     <row r="15">
@@ -942,22 +890,18 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>BDE</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0223714285714285</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1365538104962959</v>
       </c>
     </row>
     <row r="16">
@@ -977,22 +921,18 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>ACE</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0726758457229045</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.4305782101544178</v>
       </c>
     </row>
     <row r="17">
@@ -1016,18 +956,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>AF</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1043,26 +979,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>HybridKNN_RF</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>BDF</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.04698</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.385081967213115</v>
       </c>
     </row>
     <row r="19">
@@ -1078,26 +1010,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>HybridKNN_RF</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+          <t>BDF</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.025968</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.2128524590163936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>